<commit_message>
fixed bug with summery clearing appended afrer report generation
</commit_message>
<xml_diff>
--- a/dell/offline/C1VP2S2_config_report_conf_passed.xml_report.xlsx
+++ b/dell/offline/C1VP2S2_config_report_conf_passed.xml_report.xlsx
@@ -19,7 +19,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -28,7 +28,33 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">"Blinking" not equal golden setting "Off" </t>
+          <t xml:space="preserve">"Service Tag" not equal golden setting "OS System Name" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"Enabled" not equal golden setting "Disabled" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B395" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"255.255.255.0" not equal golden setting "255.255.224.0" </t>
         </r>
       </text>
     </comment>
@@ -72,6 +98,9 @@
     <t>System.Embedded.1 LCD.1#Configuration</t>
   </si>
   <si>
+    <t>failed</t>
+  </si>
+  <si>
     <t>System.Embedded.1 LCD.1#vConsoleIndication</t>
   </si>
   <si>
@@ -118,9 +147,6 @@
   </si>
   <si>
     <t>System.Embedded.1 ChassisPwrState.1#ChassisLEDState</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
   <si>
     <t>System.Embedded.1 RepositoryUpdate</t>
@@ -5391,13 +5417,13 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
@@ -5405,7 +5431,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
@@ -5413,7 +5439,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
@@ -5421,7 +5447,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
@@ -5429,7 +5455,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -5437,7 +5463,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -5445,7 +5471,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -5453,7 +5479,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -5461,7 +5487,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
@@ -5469,7 +5495,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>1</v>
@@ -5477,7 +5503,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>1</v>
@@ -5485,7 +5511,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -5493,7 +5519,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -5501,15 +5527,15 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>1</v>
@@ -5517,10 +5543,10 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -8471,8 +8497,8 @@
       <c r="A395" t="s">
         <v>396</v>
       </c>
-      <c r="B395" s="2" t="s">
-        <v>1</v>
+      <c r="B395" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="396" spans="1:2">

</xml_diff>